<commit_message>
Atualização automática de SAO_FRANCISCO_DE_PAULA.xlsx
</commit_message>
<xml_diff>
--- a/SAO_FRANCISCO_DE_PAULA.xlsx
+++ b/SAO_FRANCISCO_DE_PAULA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E8E2C71-8C5F-47A3-9C53-845A7BD050F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1989110F-A2E5-468D-B79B-8A3D96C6B08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,7 +1173,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{81984184-14D1-43C3-9F94-DB45561F94A6}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2078C63C-5274-44A1-AEA6-810E44C6F358}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1203,10 +1203,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C909A3A6-EDE9-440D-AF4F-8E90E0414980}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541DD31F-1775-49A5-8B48-FDE808A44C8B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1244,7 +1244,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B2FF37-117C-44CF-9855-B25450B73391}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CE6E19D-8103-4373-8929-F0D7E9E8EF77}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,7 +1307,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1207D5BF-8A6B-4FCC-8949-E0C5BF2224DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6478FF9A-BD1A-4953-BE93-554CB19D85D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1326,7 +1326,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E08FA7E-2C83-AFC3-B8C9-94252F21D5D7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9629CAE5-81C1-3F2B-117D-BCDC0353A1E1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1375,7 +1375,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBD8328-9252-33BE-BD67-ECD21954121F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE976C3D-41CD-E50C-9B8D-F235B3241E9E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1394,7 +1394,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62CC9D13-9CED-78D1-65B2-1F44A82DD64B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222F5AE4-836D-A7E8-96ED-B7DAA7CBCF8E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1425,7 +1425,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D2DC026-D63B-F344-6100-58767EEDDA8B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DD010AD-6A2C-1E50-B3B9-0393013E667F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1456,7 +1456,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D7FE6B6-8815-1E52-B2E2-0467CE9D442A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1E6DE7-4700-F467-019D-DB009E9CE94A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6108469-5962-4C18-9663-F08BFA195CD8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D00B0882-F775-4B86-A2D9-ED497781231B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1537,7 +1537,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC5C7ED-66F1-414A-892C-469F51ABC63F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB6D722-7386-4D9B-B216-07B4C27FAE34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,7 +1580,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D04A9B7-F9E8-460B-91CB-EAE70DCA2724}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA98F1EE-0060-4F25-B586-3026A7325BAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,7 +1893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA763350-CC21-445E-B98C-F4333618449F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A44FAF-642B-47D4-A70A-DEA19FE8839D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>